<commit_message>
justification of choices doc
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Requirements</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t xml:space="preserve">add QR code scanning </t>
+  </si>
+  <si>
+    <t>Create API for adding datasources, tags and information. Used for admin web app</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B9"/>
+  <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,35 +447,58 @@
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="B5">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="B7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
+      <c r="B8">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>8</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mongo db and docs
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27815"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\FYPRepo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew/Documents/FYPRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Requirements</t>
   </si>
@@ -54,12 +60,27 @@
   </si>
   <si>
     <t>Create API for adding datasources, tags and information. Used for admin web app</t>
+  </si>
+  <si>
+    <t>Creation of mongodb database</t>
+  </si>
+  <si>
+    <t>creation of nodejs web api</t>
+  </si>
+  <si>
+    <t>pulling of datafrom mongo db to google maps application</t>
+  </si>
+  <si>
+    <t>creation of tags and putting them into mongodb</t>
+  </si>
+  <si>
+    <t>ui/css of web app</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,19 +438,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B10"/>
+  <dimension ref="A2:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="1" max="1" width="52.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -445,7 +466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -453,7 +474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -461,7 +482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -469,7 +490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -477,7 +498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -485,7 +506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -493,12 +514,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
proposal work and delete on web app
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added edit and delete functionality to web app
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Week 1 - Sprint 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Requirements</t>
   </si>
@@ -156,6 +157,24 @@
   </si>
   <si>
     <t>current total estimate</t>
+  </si>
+  <si>
+    <t>w/c 30/01/2017</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>tutor meeting: advice on proposal, notes in proposal document</t>
+  </si>
+  <si>
+    <t>meeting with Tim B: need to talk to Steve about using Business Framework and coming into Sabisu, reviewed estimates, agreed to meet in either one or two weeks</t>
+  </si>
+  <si>
+    <t>to do: tidy up of user interface/look more professional. Tidy up code, remove anything that is redundant. Create test plan</t>
+  </si>
+  <si>
+    <t>work done: added delete and update functionality to web application, fixed bugs regarding click events, delete dialog added and overlay. Created stored procedures</t>
   </si>
 </sst>
 </file>
@@ -186,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,12 +215,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -228,9 +241,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +612,7 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="2"/>
       <c r="E5" t="s">
         <v>41</v>
       </c>
@@ -633,7 +646,7 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -642,7 +655,7 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -651,7 +664,7 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -665,7 +678,7 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -674,7 +687,7 @@
       <c r="B13">
         <v>0.2</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -683,7 +696,7 @@
       <c r="B14">
         <v>0.8</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -692,7 +705,7 @@
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -701,7 +714,7 @@
       <c r="B16">
         <v>0.2</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -710,7 +723,7 @@
       <c r="B17">
         <v>0.8</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -724,7 +737,7 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -733,7 +746,7 @@
       <c r="B20">
         <v>0.75</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -742,7 +755,7 @@
       <c r="B21">
         <v>0.75</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -751,7 +764,7 @@
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -760,7 +773,7 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -769,7 +782,7 @@
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -778,7 +791,7 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -787,7 +800,7 @@
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -796,7 +809,7 @@
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -805,7 +818,7 @@
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -814,7 +827,7 @@
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -823,7 +836,7 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -832,7 +845,7 @@
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -841,7 +854,7 @@
       <c r="B32">
         <v>2</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -850,7 +863,7 @@
       <c r="B33">
         <v>0.5</v>
       </c>
-      <c r="C33" s="5"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -859,7 +872,7 @@
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
@@ -868,7 +881,7 @@
       <c r="B35">
         <v>0.5</v>
       </c>
-      <c r="C35" s="5"/>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -877,7 +890,7 @@
       <c r="B36">
         <v>0.5</v>
       </c>
-      <c r="C36" s="5"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -886,7 +899,7 @@
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="5"/>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -895,7 +908,7 @@
       <c r="B38">
         <v>5</v>
       </c>
-      <c r="C38" s="5"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -904,7 +917,62 @@
       <c r="B39">
         <v>7</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="5">
+        <v>42765</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="e">
+        <f>VALUE(Sheet1!A5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created test plan and web app changes
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Requirements</t>
   </si>
@@ -171,10 +171,38 @@
     <t>meeting with Tim B: need to talk to Steve about using Business Framework and coming into Sabisu, reviewed estimates, agreed to meet in either one or two weeks</t>
   </si>
   <si>
-    <t>to do: tidy up of user interface/look more professional. Tidy up code, remove anything that is redundant. Create test plan</t>
-  </si>
-  <si>
     <t>work done: added delete and update functionality to web application, fixed bugs regarding click events, delete dialog added and overlay. Created stored procedures</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">to do: tidy up of user interface/look more professional. Tidy up code, remove anything that is redundant. Create test plan. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Change cards so they are fixed to location rather than pixel</t>
+    </r>
+  </si>
+  <si>
+    <t>talked to steve about using business framework, he said that it was owned by Sabic and licensed by Sabisu so I wont be able to use it. Also since I wont have access to IP21 it will be better to just have the data stored in SQL</t>
+  </si>
+  <si>
+    <t>Organised a visit to Sabisu for next Wednesday to show progress and get further advice</t>
+  </si>
+  <si>
+    <t>Created test plan for web application, most tests passed but a few bugs were found</t>
+  </si>
+  <si>
+    <t>Added more CSS and tidyed up code</t>
+  </si>
+  <si>
+    <t>Project proposal</t>
   </si>
 </sst>
 </file>
@@ -237,13 +265,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +592,7 @@
   <dimension ref="A2:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,51 +958,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="152.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="1"/>
+      <c r="C3" s="6">
         <v>42765</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="e">
-        <f>VALUE(Sheet1!A5)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>46</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6">
+        <v>42766</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
getting points within radius
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Week 1 - Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Week 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Requirements</t>
   </si>
@@ -224,6 +225,36 @@
   </si>
   <si>
     <t>finshed off project proposal</t>
+  </si>
+  <si>
+    <t>w/c 06/02/2017</t>
+  </si>
+  <si>
+    <t>Meeting with Eudes about proposal feedback and tall about getting data</t>
+  </si>
+  <si>
+    <t>Met with people from the uni to get data for the application. Log in data has potential ethical issues, engery data requires talking to ITACS</t>
+  </si>
+  <si>
+    <t>Meeting with Tim talked about making the application more generic to work with any database. No longer connecting to IP21</t>
+  </si>
+  <si>
+    <t>Proposal rework</t>
+  </si>
+  <si>
+    <t>web app rework</t>
+  </si>
+  <si>
+    <t>went into Sabisu to talk to Steve, said that making the web app more generic would work and is a good idea. He can provide me with some data from Dev Paramop database. Also said I should look into mocking the data myself</t>
+  </si>
+  <si>
+    <t>proposal hand in</t>
+  </si>
+  <si>
+    <t>web app rework, created web service for pulling data about a location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web app rework, need help getting the bounding box right. +/- 100m from current point </t>
   </si>
 </sst>
 </file>
@@ -286,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -296,6 +327,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,7 +1013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1122,4 +1154,106 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="100.109375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="7">
+        <v>42772</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D3" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D4" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="7">
+        <v>42773</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C7" s="7">
+        <v>42774</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="7">
+        <v>42775</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="7">
+        <v>42776</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="7">
+        <v>42777</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="7">
+        <v>42778</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
HTTP REQUESTSgit add .
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>Requirements</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>Given the brief for the project poster</t>
+  </si>
+  <si>
+    <t>Started work on project progress poster</t>
+  </si>
+  <si>
+    <t>still working on http requests. Volley does work as intended when the app is written in Java. Kolley is a kotlin library to use volley but is currently returning a byte array. Either rewrite the entire app in Java or see if its possible to do the requests in a java class file</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1398,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1421,7 +1427,21 @@
         <v>82</v>
       </c>
     </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>42787</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C6" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
turning changes the ui
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Week 2" sheetId="3" r:id="rId3"/>
     <sheet name="Week 3" sheetId="4" r:id="rId4"/>
     <sheet name="week 4" sheetId="5" r:id="rId5"/>
+    <sheet name="Week 5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
   <si>
     <t>Requirements</t>
   </si>
@@ -314,6 +315,27 @@
   </si>
   <si>
     <t>started designing UI elements</t>
+  </si>
+  <si>
+    <t>Project poster hand in/presentation</t>
+  </si>
+  <si>
+    <t>started work on report</t>
+  </si>
+  <si>
+    <t>created basic ui</t>
+  </si>
+  <si>
+    <t>compass implemented, reading values from the sensors</t>
+  </si>
+  <si>
+    <t>splitting received locations into north, south, east and west</t>
+  </si>
+  <si>
+    <t>possible battery drain issue</t>
+  </si>
+  <si>
+    <t>work on report</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1508,4 +1530,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="35.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="7">
+        <v>42793</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
+        <v>42794</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>42795</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>42796</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added ui images, created program to move enegery data from txt file to SQL database
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Week 3" sheetId="4" r:id="rId4"/>
     <sheet name="week 4" sheetId="5" r:id="rId5"/>
     <sheet name="Week 5" sheetId="6" r:id="rId6"/>
+    <sheet name="week 6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
   <si>
     <t>Requirements</t>
   </si>
@@ -336,6 +337,24 @@
   </si>
   <si>
     <t>work on report</t>
+  </si>
+  <si>
+    <t>grid ui created</t>
+  </si>
+  <si>
+    <t>card view implemented</t>
+  </si>
+  <si>
+    <t>testing of camera and location services</t>
+  </si>
+  <si>
+    <t>test http requests</t>
+  </si>
+  <si>
+    <t>test compass and ui</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -398,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -410,6 +429,9 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1119,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,6 +1280,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1266,7 +1293,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -1360,6 +1387,11 @@
         <v>69</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1371,7 +1403,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1438,8 +1470,8 @@
       <c r="C8" s="6">
         <v>42785</v>
       </c>
-      <c r="D8" t="s">
-        <v>76</v>
+      <c r="D8" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1450,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1526,6 +1558,11 @@
         <v>87</v>
       </c>
     </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1534,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G7"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1590,6 +1627,68 @@
         <v>95</v>
       </c>
     </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>42769</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>42770</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>42771</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="7">
+        <v>42772</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
app and report work
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="week 4" sheetId="5" r:id="rId5"/>
     <sheet name="Week 5" sheetId="6" r:id="rId6"/>
     <sheet name="week 6" sheetId="7" r:id="rId7"/>
+    <sheet name="Week 7" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
   <si>
     <t>Requirements</t>
   </si>
@@ -373,6 +374,21 @@
   </si>
   <si>
     <t>started work on pulling location data through to app</t>
+  </si>
+  <si>
+    <t>data about location pulled into web app</t>
+  </si>
+  <si>
+    <t>Graph added to app using android graph view</t>
+  </si>
+  <si>
+    <t>Location data plotted on graph</t>
+  </si>
+  <si>
+    <t>Test pulling data and displaying graph</t>
+  </si>
+  <si>
+    <t>Work on report</t>
   </si>
 </sst>
 </file>
@@ -1592,7 +1608,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1647,7 +1663,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
-        <v>42769</v>
+        <v>42797</v>
       </c>
       <c r="C8" t="s">
         <v>76</v>
@@ -1655,7 +1671,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
-        <v>42770</v>
+        <v>42798</v>
       </c>
       <c r="C9" t="s">
         <v>95</v>
@@ -1663,7 +1679,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
-        <v>42771</v>
+        <v>42799</v>
       </c>
       <c r="C10" t="s">
         <v>96</v>
@@ -1694,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1741,6 +1757,56 @@
         <v>107</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>42775</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>42776</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>42779</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
started work on offline caching
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Week 5" sheetId="6" r:id="rId6"/>
     <sheet name="week 6" sheetId="7" r:id="rId7"/>
     <sheet name="Week 7" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
   <si>
     <t>Requirements</t>
   </si>
@@ -389,6 +390,21 @@
   </si>
   <si>
     <t>Work on report</t>
+  </si>
+  <si>
+    <t>meeting with Tim, discussed using standard deviation to find outliers in data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">started work on implementing standard deviation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">implemented standard deviation, using the population version instead of sample </t>
+  </si>
+  <si>
+    <t>looking into implementing QR code scanning</t>
+  </si>
+  <si>
+    <t>issue with graph not displaying all data, cant scroll with dates</t>
   </si>
 </sst>
 </file>
@@ -1791,20 +1807,96 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C3"/>
+  <dimension ref="B3:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="7">
-        <v>42779</v>
+        <v>42807</v>
       </c>
       <c r="C3" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>42808</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>42809</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>42810</v>
+      </c>
+      <c r="C7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>42811</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>42812</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>42813</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>42814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>